<commit_message>
Hello 2023, Add Backlog,Demo 3 bow skill, add uimanager
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -1,25 +1,170 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC41D49-9B91-4BCA-9B54-8608D85C08C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+  <si>
+    <t>backlog</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Skill For Bow</t>
+  </si>
+  <si>
+    <t>Skill For Spear</t>
+  </si>
+  <si>
+    <t>Skill For Sword</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Type Of Enemy</t>
+  </si>
+  <si>
+    <t>Type Of Boss</t>
+  </si>
+  <si>
+    <t>Manager Object</t>
+  </si>
+  <si>
+    <t>có định design default boss class : tự dùng skill theo vị trí của người chơi không</t>
+  </si>
+  <si>
+    <t>Character Manager</t>
+  </si>
+  <si>
+    <t>Base Skill</t>
+  </si>
+  <si>
+    <t>Tất cả các skill implement interface này</t>
+  </si>
+  <si>
+    <t>Có thể sửa đổi thêm thắt</t>
+  </si>
+  <si>
+    <t>?%</t>
+  </si>
+  <si>
+    <t>1 nhân vật có bao nhiêu skill chủ động vs bị động?</t>
+  </si>
+  <si>
+    <t>Base Status</t>
+  </si>
+  <si>
+    <t>Chỉ số sẽ bao gồm những gì</t>
+  </si>
+  <si>
+    <t>có thiết kế khả năng duy chuyển riêng k , hay cứ tự lao vào người chơi thôi</t>
+  </si>
+  <si>
+    <t>Scene Manager</t>
+  </si>
+  <si>
+    <t>Theo dõi quá trình của màn chơi, quản lý waves quái vào sinh boss?</t>
+  </si>
+  <si>
+    <t>Character Movement</t>
+  </si>
+  <si>
+    <t>định nghĩa cách duy chuyển cho người chơi + control</t>
+  </si>
+  <si>
+    <t>Chưa viết lưu thông tin và load</t>
+  </si>
+  <si>
+    <t>UI Manager</t>
+  </si>
+  <si>
+    <t>có chia riêng ra 2 loại ui, 1 liên quan đến máu , skill, joystick, loại còn lại là chọn kĩ năng, thăng cấp chọn cộng chỉ số không</t>
+  </si>
+  <si>
+    <t>quản lý ui người chơi tương tác, đăng kí và tự gán nút,tải ảnh cho skill</t>
+  </si>
+  <si>
+    <t>Drop Manager</t>
+  </si>
+  <si>
+    <t>Quản lý những thứ ng chơi nhận được khi giết được 1 loại quái nhất định(exp, skill point)</t>
+  </si>
+  <si>
+    <t>Đăng kí skill,lưu, load thông tin cho người chơi, cho phép điều chỉnh tất cả các skill trong editor</t>
+  </si>
+  <si>
+    <t>Number Of Scene?</t>
+  </si>
+  <si>
+    <t>Start Scene</t>
+  </si>
+  <si>
+    <t>Home Scene</t>
+  </si>
+  <si>
+    <t>Scene để chọn màn giống survior.io</t>
+  </si>
+  <si>
+    <t>DeadLine</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Number Of Music Type?</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +174,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +200,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +483,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.88671875" customWidth="1"/>
+    <col min="2" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add skill garen, boss demo
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327AFF53-82FE-49C4-9FB6-799A0454E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DEDF24-5130-4055-9002-CB503D0907AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>backlog</t>
   </si>
@@ -182,16 +182,16 @@
     <t>Nam:31/01/2023</t>
   </si>
   <si>
-    <t>Tuấn:5/2/2023</t>
-  </si>
-  <si>
-    <t>Dũng:5/2/2023</t>
-  </si>
-  <si>
     <t>Nam:5/02/2023</t>
   </si>
   <si>
     <t>05/02/2023: check Deadline + giao việc design pattern + code quái</t>
+  </si>
+  <si>
+    <t>Tuấn:5/02/2023</t>
+  </si>
+  <si>
+    <t>Dũng:5/02/2023</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -597,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -608,15 +608,15 @@
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
+      <c r="B8" s="2">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
@@ -747,7 +747,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -786,7 +786,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trien khai TypeObject va Factory Pattern
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project PRU\Infinity_game\documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F70BD4-270A-4F33-A1B0-97336523FA1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F052E3-E535-48BC-B19B-374A1288FC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>backlog</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Number Of Music Type?</t>
   </si>
   <si>
-    <t>Hp,Speed,Mana</t>
-  </si>
-  <si>
     <t>2 loại quái : đến 1 tầm r đứng bắn+ lao tới</t>
   </si>
   <si>
@@ -180,10 +177,46 @@
     <t>Dũng:5/2/2023</t>
   </si>
   <si>
-    <t>Nam:5/02/2023</t>
-  </si>
-  <si>
     <t>05/02/2023: check Deadline + giao việc design pattern + code quái</t>
+  </si>
+  <si>
+    <t>Hp,Speed,atk</t>
+  </si>
+  <si>
+    <t>Being Attack, Attack, setter, getter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save Game Manager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tắt game , thoát từ menu thì save lại lv nhân vật, </t>
+  </si>
+  <si>
+    <t>wave mấy, hp hiện tại quái, nhân vật, vị trí quái</t>
+  </si>
+  <si>
+    <t>làm màn chọn skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lúc chọn màn chơi thì cho ng chơi chọn 3 kĩ năng </t>
+  </si>
+  <si>
+    <t>Nam 15/02</t>
+  </si>
+  <si>
+    <t>Dũng 15/02</t>
+  </si>
+  <si>
+    <t>Nam:15/02/2023</t>
+  </si>
+  <si>
+    <t>Tuấn 15/02</t>
+  </si>
+  <si>
+    <t>State Manager</t>
+  </si>
+  <si>
+    <t>Thêm vào mọi loại quái để checkAvailableStage và thực thi</t>
   </si>
 </sst>
 </file>
@@ -199,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,11 +264,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,25 +550,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.90625" customWidth="1"/>
-    <col min="2" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="78.453125" customWidth="1"/>
+    <col min="1" max="1" width="52.88671875" customWidth="1"/>
+    <col min="2" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -545,14 +585,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -567,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -575,13 +615,13 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -589,10 +629,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -600,10 +640,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -611,32 +651,38 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -644,13 +690,13 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -658,15 +704,15 @@
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -681,7 +727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -692,7 +738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -707,78 +753,114 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>52</v>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trien khai state design pattern
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F052E3-E535-48BC-B19B-374A1288FC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2985EABA-7D85-4B7E-8BC9-91D24209AF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>backlog</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Thêm vào mọi loại quái để checkAvailableStage và thực thi</t>
+  </si>
+  <si>
+    <t>Design Pattern Applied: Factory, Object Pool, Type Object, Observer</t>
+  </si>
+  <si>
+    <t>All Apply :  Factory, Object Pool, Type Object, Observer, State, Singleton</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,8 +617,8 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
+      <c r="B5" s="2">
+        <v>0.9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>49</v>
@@ -625,8 +631,8 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
+      <c r="B6" s="2">
+        <v>0.9</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>48</v>
@@ -636,8 +642,8 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
+      <c r="B7" s="2">
+        <v>0.9</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>47</v>
@@ -647,8 +653,8 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
+      <c r="B8" s="2">
+        <v>0.9</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -686,8 +692,8 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
+      <c r="B11" s="2">
+        <v>0.9</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
@@ -700,8 +706,8 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
+      <c r="B12" s="2">
+        <v>0.9</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>42</v>
@@ -772,7 +778,9 @@
       <c r="A18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>0.9</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>63</v>
@@ -861,6 +869,16 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chinh sua state cho boss,creep, them cong thuc gay sat thuong cho quai,them co che spawn cho 2 spawner , them kiem soat man choi cho scenemanager
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2985EABA-7D85-4B7E-8BC9-91D24209AF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA965F76-CDDF-48EB-AF37-A681CAFFAC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>backlog</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Scene Manager</t>
   </si>
   <si>
-    <t>Theo dõi quá trình của màn chơi, quản lý waves quái vào sinh boss?</t>
-  </si>
-  <si>
     <t>Character Movement</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Tuấn/26/01</t>
   </si>
   <si>
-    <t>4 màn : vs 2 màn map khác nhau</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Dũng:5/2/2023</t>
   </si>
   <si>
-    <t>05/02/2023: check Deadline + giao việc design pattern + code quái</t>
-  </si>
-  <si>
     <t>Hp,Speed,atk</t>
   </si>
   <si>
@@ -223,6 +214,33 @@
   </si>
   <si>
     <t>All Apply :  Factory, Object Pool, Type Object, Observer, State, Singleton</t>
+  </si>
+  <si>
+    <t>bảng record kỉ lục</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Nam: 09/03</t>
+  </si>
+  <si>
+    <t>Nam: 09/03(Tạo UI)</t>
+  </si>
+  <si>
+    <t>Menu trong màn chơi</t>
+  </si>
+  <si>
+    <t>Dừng game, chuyển ra menu chính, chỉnh nhạc, exit</t>
+  </si>
+  <si>
+    <t>1 màn</t>
+  </si>
+  <si>
+    <t>?%(Bỏ)</t>
+  </si>
+  <si>
+    <t>Theo dõi quá trình của màn chơi, quản lý waves creep và sinh boss?</t>
   </si>
 </sst>
 </file>
@@ -559,7 +577,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -621,7 +639,7 @@
         <v>0.9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -635,7 +653,7 @@
         <v>0.9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -646,24 +664,24 @@
         <v>0.9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2">
         <v>0.9</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -674,10 +692,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -696,7 +714,7 @@
         <v>0.9</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -710,7 +728,7 @@
         <v>0.9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -727,74 +745,74 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
+      <c r="B15" s="2">
+        <v>0.5</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2">
         <v>0.3</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2">
         <v>0.9</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -804,81 +822,102 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2">
         <v>0.7</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hoan chinh creepStateManager, bossStateManager, them boss 1 state affect UI
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA965F76-CDDF-48EB-AF37-A681CAFFAC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22052B56-EF57-4AE3-8F9A-44E215FB69AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>backlog</t>
   </si>
@@ -192,9 +192,6 @@
     <t xml:space="preserve">lúc chọn màn chơi thì cho ng chơi chọn 3 kĩ năng </t>
   </si>
   <si>
-    <t>Nam 15/02</t>
-  </si>
-  <si>
     <t>Dũng 15/02</t>
   </si>
   <si>
@@ -241,6 +238,15 @@
   </si>
   <si>
     <t>Theo dõi quá trình của màn chơi, quản lý waves creep và sinh boss?</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Người chơi gây dame cho quái</t>
+  </si>
+  <si>
+    <t>Quái gây dame cho người chơi</t>
   </si>
 </sst>
 </file>
@@ -574,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,7 +765,7 @@
         <v>0.5</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,9 +787,11 @@
       <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>51</v>
@@ -794,14 +802,14 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2">
         <v>0.9</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -825,7 +833,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -836,7 +844,7 @@
         <v>0.7</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -844,7 +852,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
@@ -863,7 +871,7 @@
         <v>0.5</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -876,13 +884,13 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -890,10 +898,10 @@
         <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>54</v>
@@ -901,23 +909,38 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug ( set 0 voi 1 loai trong creep factory), trien khai ham gay sat thuong cho quai tu ki nang, them ki nang blackholeshot cho nguoi choi, fix bug gimball lock
</commit_message>
<xml_diff>
--- a/documentations/Phân chia công việc.XLSX
+++ b/documentations/Phân chia công việc.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRU211\My2dGame\Infinity_game\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22052B56-EF57-4AE3-8F9A-44E215FB69AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5D1AD-B59A-45F8-BCC2-7753DDBA45E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>backlog</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Quái gây dame cho người chơi</t>
+  </si>
+  <si>
+    <t>hồi chiêu cho kĩ năng</t>
+  </si>
+  <si>
+    <t>mở khóa bảng chọn kĩ năng theo kỉ lục đạt được</t>
   </si>
 </sst>
 </file>
@@ -583,7 +589,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,6 +939,16 @@
         <v>73</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>60</v>

</xml_diff>